<commit_message>
before ahsraf edit accuracy
</commit_message>
<xml_diff>
--- a/Bubble_Sheet_Student_Results.xlsx
+++ b/Bubble_Sheet_Student_Results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CW39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -974,6 +974,3190 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1998876</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" t="n">
+        <v>1</v>
+      </c>
+      <c r="W17" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0101</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>9170044</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1</v>
+      </c>
+      <c r="V19" t="n">
+        <v>1</v>
+      </c>
+      <c r="W19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>9998</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>4521</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" t="n">
+        <v>1</v>
+      </c>
+      <c r="W21" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0011</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1</v>
+      </c>
+      <c r="U22" t="n">
+        <v>1</v>
+      </c>
+      <c r="V22" t="n">
+        <v>1</v>
+      </c>
+      <c r="W22" t="n">
+        <v>1</v>
+      </c>
+      <c r="X22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>9643435</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1</v>
+      </c>
+      <c r="V23" t="n">
+        <v>1</v>
+      </c>
+      <c r="W23" t="n">
+        <v>1</v>
+      </c>
+      <c r="X23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>9043435</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" t="n">
+        <v>1</v>
+      </c>
+      <c r="V24" t="n">
+        <v>1</v>
+      </c>
+      <c r="W24" t="n">
+        <v>1</v>
+      </c>
+      <c r="X24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>9999996</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1</v>
+      </c>
+      <c r="V25" t="n">
+        <v>1</v>
+      </c>
+      <c r="W25" t="n">
+        <v>1</v>
+      </c>
+      <c r="X25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>9999996</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1</v>
+      </c>
+      <c r="V26" t="n">
+        <v>1</v>
+      </c>
+      <c r="W26" t="n">
+        <v>1</v>
+      </c>
+      <c r="X26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0123456</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1</v>
+      </c>
+      <c r="V27" t="n">
+        <v>1</v>
+      </c>
+      <c r="W27" t="n">
+        <v>1</v>
+      </c>
+      <c r="X27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1111111</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>1</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1</v>
+      </c>
+      <c r="V28" t="n">
+        <v>1</v>
+      </c>
+      <c r="W28" t="n">
+        <v>1</v>
+      </c>
+      <c r="X28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1111111</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1</v>
+      </c>
+      <c r="V29" t="n">
+        <v>1</v>
+      </c>
+      <c r="W29" t="n">
+        <v>1</v>
+      </c>
+      <c r="X29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>6666669</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1</v>
+      </c>
+      <c r="V30" t="n">
+        <v>1</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1</v>
+      </c>
+      <c r="X30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>3333333</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2222222</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0000001</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1</v>
+      </c>
+      <c r="V33" t="n">
+        <v>1</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2089</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>5505</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0886</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1</v>
+      </c>
+      <c r="P37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0991</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0034</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>